<commit_message>
Fast auto download all zip assignments using threads
</commit_message>
<xml_diff>
--- a/Internshala-Python-Users.xlsx
+++ b/Internshala-Python-Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Python\Web-Automate-Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6263F361-AD97-4A85-9AEC-42D9957B1992}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E70254B6-7B69-4E29-8490-B16C93817301}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,6 +1014,7 @@
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" customWidth="1"/>
     <col min="4" max="4" width="88.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1630,7 +1631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1638,6 +1641,7 @@
     <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="85.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Posting data online complete by fetching inputs from XL
</commit_message>
<xml_diff>
--- a/Internshala-Python-Users.xlsx
+++ b/Internshala-Python-Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Python\Web-Automate-Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E70254B6-7B69-4E29-8490-B16C93817301}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{77C019AC-CC5B-4BB4-A1B2-9DEB4D2845C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="231">
   <si>
     <t>Name</t>
   </si>
@@ -465,6 +465,24 @@
     <t>https://trainings.internshala.com/uploads/python/uploads/projects/v_2/865979/5e78b7b8cdc9c.rar</t>
   </si>
   <si>
+    <t>devanand.gupta@gmail.com</t>
+  </si>
+  <si>
+    <t>2020-03-24 18:00:05</t>
+  </si>
+  <si>
+    <t>https://trainings.internshala.com/uploads/python/uploads/projects/v_2/826406/5e79fd4dbf3b3.rar</t>
+  </si>
+  <si>
+    <t>Somjitm786@gmail.com</t>
+  </si>
+  <si>
+    <t>2020-03-24 19:26:20</t>
+  </si>
+  <si>
+    <t>https://trainings.internshala.com/uploads/python/uploads/projects/v_2/855420/5e7a1184b4774.rar</t>
+  </si>
+  <si>
     <t>anulekhapolati246@gmail.com</t>
   </si>
   <si>
@@ -477,18 +495,6 @@
     <t>https://trainings.internshala.com/uploads/python/uploads/projects/v_2/756282/5dda57475447c.zip</t>
   </si>
   <si>
-    <t>akash.ravi@internshala.com</t>
-  </si>
-  <si>
-    <t>2019-12-09</t>
-  </si>
-  <si>
-    <t>2019-12-16 13:04:48</t>
-  </si>
-  <si>
-    <t>https://trainings.internshala.com/uploads/python/uploads/projects/v_2/814431/5df733986aabf.zip</t>
-  </si>
-  <si>
     <t>ashish.mp139@gmail.com</t>
   </si>
   <si>
@@ -652,16 +658,80 @@
   </si>
   <si>
     <t>https://trainings.internshala.com/uploads/python/uploads/projects/v_2/870456/5e74d971c7f83.zip</t>
+  </si>
+  <si>
+    <t>No files submitted</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Available points not displayed, End cases unchecked, Good UI, Database tables not proper</t>
+  </si>
+  <si>
+    <t>Work on UI, Improper error checking, Players removable even after saving, Evaluate score not working</t>
+  </si>
+  <si>
+    <t>Incomplete, No database, No methods implemented</t>
+  </si>
+  <si>
+    <t>Work on UI, Errors have not been checked, Available points becomes negative, databses should be more organized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plagiarized </t>
+  </si>
+  <si>
+    <t>Code not running</t>
+  </si>
+  <si>
+    <t>Work on UI, Do not allow players to be moved back when opening team</t>
+  </si>
+  <si>
+    <t>Database not complete, Improve UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plagiarized </t>
+  </si>
+  <si>
+    <t>Great UI, Proper error checks, Database connection working, Add comments to code</t>
+  </si>
+  <si>
+    <t>Improper files</t>
+  </si>
+  <si>
+    <t>Missing Modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plagiarized, UI crashes </t>
+  </si>
+  <si>
+    <t>plagiarized</t>
+  </si>
+  <si>
+    <t>UI crashes on interacting with elements</t>
+  </si>
+  <si>
+    <t>Nicely done, All elements and database working, fill up all the match tables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -675,12 +745,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -692,16 +767,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1002,22 +1080,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="88.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="83.33203125" customWidth="1"/>
+    <col min="6" max="6" width="113" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1030,9 +1108,15 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="E1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -1044,8 +1128,14 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1058,9 +1148,15 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
@@ -1072,9 +1168,15 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
@@ -1086,8 +1188,14 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1100,8 +1208,14 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1114,8 +1228,14 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1128,8 +1248,14 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1142,8 +1268,14 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1156,8 +1288,14 @@
       <c r="D10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1170,8 +1308,14 @@
       <c r="D11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1184,8 +1328,14 @@
       <c r="D12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1198,8 +1348,14 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1212,9 +1368,15 @@
       <c r="D14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B15" t="s">
@@ -1226,8 +1388,14 @@
       <c r="D15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1240,8 +1408,14 @@
       <c r="D16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1254,8 +1428,14 @@
       <c r="D17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1268,8 +1448,14 @@
       <c r="D18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1282,8 +1468,14 @@
       <c r="D19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>85</v>
+      </c>
+      <c r="F19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1296,9 +1488,15 @@
       <c r="D20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
@@ -1310,8 +1508,14 @@
       <c r="D21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1324,8 +1528,14 @@
       <c r="D22" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1338,8 +1548,14 @@
       <c r="D23" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1352,8 +1568,14 @@
       <c r="D24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -1366,8 +1588,14 @@
       <c r="D25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1380,8 +1608,14 @@
       <c r="D26" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -1394,8 +1628,14 @@
       <c r="D27" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1408,8 +1648,14 @@
       <c r="D28" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -1422,8 +1668,14 @@
       <c r="D29" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -1436,8 +1688,14 @@
       <c r="D30" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1450,8 +1708,14 @@
       <c r="D31" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -1464,8 +1728,14 @@
       <c r="D32" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -1478,8 +1748,14 @@
       <c r="D33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>65</v>
+      </c>
+      <c r="F33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -1492,8 +1768,14 @@
       <c r="D34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -1506,8 +1788,14 @@
       <c r="D35" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -1520,9 +1808,15 @@
       <c r="D36" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="E36">
+        <v>40</v>
+      </c>
+      <c r="F36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B37" t="s">
@@ -1535,8 +1829,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B38" t="s">
@@ -1549,8 +1843,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B39" t="s">
@@ -1563,8 +1857,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B40" t="s">
@@ -1577,8 +1871,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B41" t="s">
@@ -1591,8 +1885,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B42" t="s">
@@ -1605,8 +1899,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B43" t="s">
@@ -1619,9 +1913,41 @@
         <v>146</v>
       </c>
     </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{9C81B191-4559-46C5-A823-7D8E345D3671}"/>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{41717839-E13A-44BB-A1DB-E6E72900E4CD}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{2759FF5E-9C15-4679-8BDF-CE6E66CE7EDC}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{5DBFEC2B-EEBD-45BA-A9AA-179ADCEFA6F4}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{8438C701-CB69-4718-997B-E2BB431620AA}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{8CFD60A3-2C19-4E20-A9BF-70C151E9E683}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1629,19 +1955,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="85.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="88.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1660,450 +1985,436 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B22" t="s">
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D23" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D24" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D26" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D30" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D31" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D32" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>207</v>
-      </c>
-      <c r="B33" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" t="s">
-        <v>208</v>
-      </c>
-      <c r="D33" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>